<commit_message>
ods to xlsx and one more chart
</commit_message>
<xml_diff>
--- a/Results/ResultsTest1.xlsx
+++ b/Results/ResultsTest1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ParticleChromo3D\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC878E8-E2E4-417F-8899-B0D37905EF8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2975E821-A43B-48F3-9A2E-630D2774EF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="3345" windowWidth="17355" windowHeight="15435" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="3345" windowWidth="17355" windowHeight="15435" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameterChoiceForBestAlpha" sheetId="1" r:id="rId1"/>
@@ -54,35 +54,17 @@
     <definedName name="_xlchart.v1.33" hidden="1">'consistency-1MB'!$R$2:$R$436</definedName>
     <definedName name="_xlchart.v1.34" hidden="1">'consistency-1MB'!$S$1</definedName>
     <definedName name="_xlchart.v1.35" hidden="1">'consistency-1MB'!$S$2:$S$436</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'consistency-1MB'!$K$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'consistency-1MB'!$K$2:$K$436</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'consistency-1MB'!$L$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'consistency-1MB'!$L$2:$L$436</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'consistency-500kb'!$K$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'consistency-500kb'!$K$2:$K$2188</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'consistency-500kb'!$L$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'consistency-500kb'!$L$2:$L$2188</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'consistency-1MB'!$M$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'consistency-1MB'!$M$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'consistency-1MB'!$M$2:$M$436</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'consistency-1MB'!$N$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'consistency-1MB'!$N$2:$N$436</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'consistency-1MB'!$O$1</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'consistency-1MB'!$O$2:$O$436</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'consistency-1MB'!$P$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'consistency-1MB'!$P$2:$P$436</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'consistency-1MB'!$Q$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'consistency-1MB'!$Q$2:$Q$436</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'consistency-500kb'!$M$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'consistency-500kb'!$M$2:$M$2188</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'consistency-500kb'!$N$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'consistency-500kb'!$N$2:$N$2188</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'consistency-1MB'!$M$2:$M$436</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'consistency-1MB'!$R$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">'consistency-1MB'!$R$2:$R$436</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">'consistency-1MB'!$S$1</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">'consistency-1MB'!$S$2:$S$436</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">'consistency-500kb'!$K$1</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">'consistency-500kb'!$K$2:$K$2188</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">'consistency-500kb'!$L$1</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">'consistency-500kb'!$L$2:$L$2188</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">'consistency-500kb'!$M$1</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">'consistency-500kb'!$M$2:$M$2188</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'consistency-1MB'!$N$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">'consistency-500kb'!$N$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">'consistency-500kb'!$N$2:$N$2188</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'consistency-1MB'!$N$2:$N$436</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'consistency-1MB'!$O$1</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">'consistency-1MB'!$O$2:$O$436</definedName>
@@ -1781,6 +1763,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -2641,6 +2629,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -3050,6 +3044,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -3477,6 +3477,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -3904,6 +3910,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -4313,6 +4325,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -4730,6 +4748,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5147,6 +5171,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6058,6 +6088,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6446,6 +6482,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6833,6 +6875,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -7220,6 +7268,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -13285,47 +13339,47 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.39</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.45</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.47</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.49</cx:f>
+        <cx:f>_xlchart.v1.31</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.51</cx:f>
+        <cx:f>_xlchart.v1.33</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.53</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -13363,7 +13417,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E74A45CE-B0CE-4284-AD37-4930D0C01BCC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.36</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>chr1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13376,7 +13430,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4609CE68-5C56-4848-9F7F-D5A847B5B531}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.38</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>chr2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13389,7 +13443,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B572AA01-5165-4463-9556-6071969C41E6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>chr5</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13402,7 +13456,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{0C22D4F5-4BCE-466F-A466-25E8A48B3543}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.42</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>chr10</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13415,7 +13469,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8CB4A5A0-6872-4707-A7D7-7DC65CC83719}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.44</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>chr15</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13428,7 +13482,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B7B94A64-8346-49DD-9086-43559FCFD78D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.46</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>chr19</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13441,7 +13495,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D3994CC7-33C9-4B5A-B63C-1071FA6518E9}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.48</cx:f>
+              <cx:f>_xlchart.v1.30</cx:f>
               <cx:v>chr20</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13454,7 +13508,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{BBDBC415-1A60-4213-BA90-2D8510942363}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.50</cx:f>
+              <cx:f>_xlchart.v1.32</cx:f>
               <cx:v>chr21</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13467,7 +13521,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{380E1564-8E15-44AC-BDEF-5F3A534B83E8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.52</cx:f>
+              <cx:f>_xlchart.v1.34</cx:f>
               <cx:v>chr22</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13546,22 +13600,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.55</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.57</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.59</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.61</cx:f>
+        <cx:f>_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -13599,7 +13653,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FC0FDC28-34D3-4A75-A532-D3429BECE732}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.54</cx:f>
+              <cx:f>_xlchart.v1.36</cx:f>
               <cx:v>chr1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13612,7 +13666,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FDF954FF-C90D-448A-BAC7-9EB7101C5083}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.56</cx:f>
+              <cx:f>_xlchart.v1.38</cx:f>
               <cx:v>chr10</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13625,7 +13679,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{37A695BD-6086-4712-9A72-01FE7C456FFF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.58</cx:f>
+              <cx:f>_xlchart.v1.40</cx:f>
               <cx:v>chr19</cx:v>
             </cx:txData>
           </cx:tx>
@@ -13638,7 +13692,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{588D971C-E56B-4A45-8E9E-CFAF2A37CD1E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.60</cx:f>
+              <cx:f>_xlchart.v1.42</cx:f>
               <cx:v>chr22</cx:v>
             </cx:txData>
           </cx:tx>
@@ -15627,16 +15681,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -15672,7 +15726,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4343400" y="2205037"/>
+              <a:off x="9753600" y="2947987"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -16677,8 +16731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16897,8 +16951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C79" sqref="C76:C79"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -17546,8 +17600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V436"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -30437,8 +30491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q2188"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -44356,7 +44410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>

</xml_diff>

<commit_message>
add HSA data set
</commit_message>
<xml_diff>
--- a/Results/ResultsTest1.xlsx
+++ b/Results/ResultsTest1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ParticleChromo3D\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2975E821-A43B-48F3-9A2E-630D2774EF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F93DC-A968-4A9C-B645-29BD4F250E22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="3345" windowWidth="17355" windowHeight="15435" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="3345" windowWidth="25215" windowHeight="15435" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameterChoiceForBestAlpha" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t>alpha</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>spearman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c1 </t>
   </si>
   <si>
     <t>This is the key chart</t>
@@ -338,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -374,6 +371,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -389,7 +395,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,6 +433,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4391,6 +4405,639 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SCC at Different Local</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Confidences vs Global Confidence</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coeffecient_test!$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$1:$V$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$2:$V$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.5435310430800803E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.101530293795098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.105514742244953</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3353-433E-92B9-8B98FE1A49EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coeffecient_test!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$1:$V$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$3:$V$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.1732378554561405E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.128296807618589</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37213812496097398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3353-433E-92B9-8B98FE1A49EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coeffecient_test!$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$1:$V$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.99377130598532104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99672801553520796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99620063830389705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3353-433E-92B9-8B98FE1A49EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1143806703"/>
+        <c:axId val="1143802543"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1143806703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Global Confidence</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1143802543"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1143802543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>SCC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1143806703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
     <c:title>
@@ -4742,429 +5389,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="514562352"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-      </c:dTable>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9528" cap="flat">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-        <a:lnSpc>
-          <a:spcPct val="100000"/>
-        </a:lnSpc>
-        <a:spcBef>
-          <a:spcPts val="0"/>
-        </a:spcBef>
-        <a:spcAft>
-          <a:spcPts val="0"/>
-        </a:spcAft>
-        <a:tabLst/>
-        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Calibri"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>PCC Average Between 30 Structures per Chromosome</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'consistency-1MB'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>chr1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>chr2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>chr5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>chr10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>chr15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>chr19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>chr20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>chr21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>chr22</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'consistency-1MB'!$D$2:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.99489709744798105</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99962796415937605</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99977975691179399</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.99742718617565596</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.98940425891647599</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.99960656313853502</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.987824364481382</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.99541762961091995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.99906937831635301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-89E6-469B-B00C-B062BCA1F243}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="514559440"/>
-        <c:axId val="514540304"/>
-      </c:barChart>
-      <c:valAx>
-        <c:axId val="514540304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9528" cap="flat">
-              <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Axis Title</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="514559440"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="514559440"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Axis Title</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9528" cap="flat">
-            <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="514540304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5766,6 +5990,429 @@
                 <a:uFillTx/>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
+              <a:t>PCC Average Between 30 Structures per Chromosome</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'consistency-1MB'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>chr1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>chr2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chr5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>chr10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>chr15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>chr19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>chr20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>chr21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>chr22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'consistency-1MB'!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.99489709744798105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99962796415937605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99977975691179399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99742718617565596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98940425891647599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99960656313853502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.987824364481382</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99541762961091995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99906937831635301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89E6-469B-B00C-B062BCA1F243}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="514559440"/>
+        <c:axId val="514540304"/>
+      </c:barChart>
+      <c:valAx>
+        <c:axId val="514540304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9528" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Axis Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514559440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="514559440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Axis Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9528" cap="flat">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514540304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9528" cap="flat">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+        <a:lnSpc>
+          <a:spcPct val="100000"/>
+        </a:lnSpc>
+        <a:spcBef>
+          <a:spcPts val="0"/>
+        </a:spcBef>
+        <a:spcAft>
+          <a:spcPts val="0"/>
+        </a:spcAft>
+        <a:tabLst/>
+        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Calibri"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
               <a:t>TM-Score Average Between 30 Structure per Chromosome</a:t>
             </a:r>
           </a:p>
@@ -6150,7 +6797,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6544,7 +7191,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6937,7 +7584,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7330,7 +7977,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8580,7 +9227,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -13826,7 +14473,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14341,7 +15531,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15376,10 +16566,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161921</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133346</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6121816" cy="3443081"/>
     <xdr:graphicFrame macro="">
@@ -15405,6 +16595,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2260126E-C95B-43B3-A23D-AFF637E86EE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16949,10 +18175,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:V83"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16961,7 +18187,7 @@
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -16990,7 +18216,7 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
@@ -17001,8 +18227,17 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="T1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U1">
+        <v>2.5</v>
+      </c>
+      <c r="V1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -17031,20 +18266,35 @@
         <v>0.99837607469027201</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="M2" s="5">
+      <c r="M2">
+        <v>0.3</v>
+      </c>
+      <c r="N2">
+        <v>0.1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>8.3145397809773702E-2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>6.6322647822716504E-2</v>
+      </c>
+      <c r="S2" s="5">
         <v>0.5</v>
       </c>
-      <c r="N2" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0.99689891449684798</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0.99672801553520796</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="T2" s="5">
+        <f>P3</f>
+        <v>7.5435310430800803E-2</v>
+      </c>
+      <c r="U2" s="5">
+        <f>P4</f>
+        <v>0.101530293795098</v>
+      </c>
+      <c r="V2" s="5">
+        <f>P5</f>
+        <v>0.105514742244953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="7">
         <v>0.3</v>
       </c>
@@ -17076,19 +18326,34 @@
       </c>
       <c r="K3" s="8"/>
       <c r="M3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="N3">
-        <v>2.5</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0.99659953493572395</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0.99620063830389705</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>0.4</v>
+      </c>
+      <c r="O3" s="1">
+        <v>9.5653206420151904E-2</v>
+      </c>
+      <c r="P3" s="1">
+        <v>7.5435310430800803E-2</v>
+      </c>
+      <c r="S3">
+        <v>0.7</v>
+      </c>
+      <c r="T3" s="5">
+        <f>P6</f>
+        <v>8.1732378554561405E-2</v>
+      </c>
+      <c r="U3" s="5">
+        <f>P7</f>
+        <v>0.128296807618589</v>
+      </c>
+      <c r="V3" s="5">
+        <f>P8</f>
+        <v>0.37213812496097398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>0.6</v>
       </c>
@@ -17116,20 +18381,35 @@
       <c r="J4" s="5">
         <v>0.99837607469027201</v>
       </c>
-      <c r="M4" s="5">
-        <v>0.5</v>
+      <c r="M4">
+        <v>0.3</v>
       </c>
       <c r="N4">
-        <v>2.8</v>
-      </c>
-      <c r="O4" s="5">
-        <v>2.5800494948756799E-2</v>
-      </c>
-      <c r="P4" s="5">
-        <v>1.7421163822083498E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>0.7</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.124147814037815</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.101530293795098</v>
+      </c>
+      <c r="S4">
+        <v>0.9</v>
+      </c>
+      <c r="T4" s="5">
+        <f>P9</f>
+        <v>0.99377130598532104</v>
+      </c>
+      <c r="U4" s="5">
+        <f>P19</f>
+        <v>0.99672801553520796</v>
+      </c>
+      <c r="V4" s="5">
+        <f>P20</f>
+        <v>0.99620063830389705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>0.9</v>
       </c>
@@ -17152,19 +18432,19 @@
         <v>2.5</v>
       </c>
       <c r="M5">
-        <v>0.7</v>
-      </c>
-      <c r="N5" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0.99844535101737397</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0.99846462103771205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>0.3</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.12666432036703101</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.105514742244953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>1.2</v>
       </c>
@@ -17187,19 +18467,19 @@
         <v>2.5</v>
       </c>
       <c r="M6">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="N6">
-        <v>2.5</v>
-      </c>
-      <c r="O6" s="5">
-        <v>1.6894316798075602E-2</v>
-      </c>
-      <c r="P6" s="5">
-        <v>1.26692786830521E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>1.3</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.10290602252389799</v>
+      </c>
+      <c r="P6" s="1">
+        <v>8.1732378554561405E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -17222,19 +18502,19 @@
         <v>2.5</v>
       </c>
       <c r="M7">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="N7">
-        <v>2.8</v>
-      </c>
-      <c r="O7" s="5">
-        <v>4.8827333114792197E-2</v>
-      </c>
-      <c r="P7" s="5">
-        <v>3.7434444673984997E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>1.6</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.17208333762880801</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.128296807618589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>1.9</v>
       </c>
@@ -17257,19 +18537,19 @@
         <v>2.5</v>
       </c>
       <c r="M8">
-        <v>0.9</v>
-      </c>
-      <c r="N8" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O8" s="5">
-        <v>0.99879633533495804</v>
-      </c>
-      <c r="P8" s="5">
-        <v>0.99868591146533103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>0.3</v>
+      </c>
+      <c r="N8">
+        <v>1.9</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.45620814069263199</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.37213812496097398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>0.3</v>
       </c>
@@ -17292,19 +18572,19 @@
         <v>2.8</v>
       </c>
       <c r="M9">
-        <v>0.9</v>
-      </c>
-      <c r="N9">
-        <v>2.5</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2.2597942669239202E-2</v>
-      </c>
-      <c r="P9" s="5">
-        <v>2.0561717472259499E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>0.3</v>
+      </c>
+      <c r="N9" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.99429792923667704</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.99377130598532104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>0.3</v>
       </c>
@@ -17336,19 +18616,19 @@
       </c>
       <c r="K10" s="8"/>
       <c r="M10">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="N10">
-        <v>2.8</v>
-      </c>
-      <c r="O10" s="5">
-        <v>2.4694577912838599E-2</v>
-      </c>
-      <c r="P10" s="5">
-        <v>2.48559342758627E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>2.5</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0.99820301162700098</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0.99814338881887299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>0.3</v>
       </c>
@@ -17371,8 +18651,20 @@
         <v>2.8</v>
       </c>
       <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="M11">
+        <v>0.3</v>
+      </c>
+      <c r="N11">
+        <v>2.8</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0.99298009111866203</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0.99216247324951001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>0.3</v>
       </c>
@@ -17394,8 +18686,16 @@
       <c r="H12" s="1">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="M12" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>0.3</v>
       </c>
@@ -17417,8 +18717,14 @@
       <c r="H13" s="1">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="M13" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>0.3</v>
       </c>
@@ -17440,8 +18746,14 @@
       <c r="H14" s="1">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="M14" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N14">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>0.3</v>
       </c>
@@ -17463,8 +18775,14 @@
       <c r="H15" s="1">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="M15" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>0.3</v>
       </c>
@@ -17480,8 +18798,14 @@
       <c r="E16" s="1">
         <v>26.636332184034099</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="M16" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N16">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>0.3</v>
       </c>
@@ -17497,8 +18821,14 @@
       <c r="E17" s="1">
         <v>25.458332387009602</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="M17" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>0.3</v>
       </c>
@@ -17514,15 +18844,270 @@
       <c r="E18" s="1">
         <v>26.038569260682301</v>
       </c>
+      <c r="M18" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N18">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="M19" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N19" s="22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O19" s="22">
+        <v>0.99689891449684798</v>
+      </c>
+      <c r="P19" s="22">
+        <v>0.99672801553520796</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="M20">
+        <v>0.5</v>
+      </c>
+      <c r="N20">
+        <v>2.5</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0.99659953493572395</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0.99620063830389705</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="M21" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="N21">
+        <v>2.8</v>
+      </c>
+      <c r="O21" s="5">
+        <v>2.5800494948756799E-2</v>
+      </c>
+      <c r="P21" s="5">
+        <v>1.7421163822083498E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="M22" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="N22" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="M23">
+        <v>0.7</v>
+      </c>
+      <c r="N23">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="M24">
+        <v>0.7</v>
+      </c>
+      <c r="N24">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="M25">
+        <v>0.7</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="M26">
+        <v>0.7</v>
+      </c>
+      <c r="N26">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="M27">
+        <v>0.7</v>
+      </c>
+      <c r="N27">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="M28">
+        <v>0.7</v>
+      </c>
+      <c r="N28">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="M29">
+        <v>0.7</v>
+      </c>
+      <c r="N29" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O29" s="5">
+        <v>0.99844535101737397</v>
+      </c>
+      <c r="P29" s="5">
+        <v>0.99846462103771205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="M30">
+        <v>0.7</v>
+      </c>
+      <c r="N30">
+        <v>2.5</v>
+      </c>
+      <c r="O30" s="5">
+        <v>1.6894316798075602E-2</v>
+      </c>
+      <c r="P30" s="5">
+        <v>1.26692786830521E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="M31">
+        <v>0.7</v>
+      </c>
+      <c r="N31">
+        <v>2.8</v>
+      </c>
+      <c r="O31" s="5">
+        <v>4.8827333114792197E-2</v>
+      </c>
+      <c r="P31" s="5">
+        <v>3.7434444673984997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="M32" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="N32" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+    </row>
+    <row r="33" spans="13:22">
+      <c r="M33" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N33">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="13:22">
+      <c r="M34" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N34">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="35" spans="13:22">
+      <c r="M35" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+    </row>
+    <row r="36" spans="13:22">
+      <c r="M36" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N36">
+        <v>1.3</v>
+      </c>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+    </row>
+    <row r="37" spans="13:22">
+      <c r="M37" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N37">
+        <v>1.6</v>
+      </c>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+    </row>
+    <row r="38" spans="13:22">
+      <c r="M38" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N38">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="39" spans="13:22">
+      <c r="M39">
+        <v>0.9</v>
+      </c>
+      <c r="N39" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O39" s="5">
+        <v>0.99879633533495804</v>
+      </c>
+      <c r="P39" s="5">
+        <v>0.99868591146533103</v>
+      </c>
+    </row>
+    <row r="40" spans="13:22">
+      <c r="M40">
+        <v>0.9</v>
+      </c>
+      <c r="N40">
+        <v>2.5</v>
+      </c>
+      <c r="O40" s="5">
+        <v>2.2597942669239202E-2</v>
+      </c>
+      <c r="P40" s="5">
+        <v>2.0561717472259499E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="13:22">
+      <c r="M41">
+        <v>0.9</v>
+      </c>
+      <c r="N41">
+        <v>2.8</v>
+      </c>
+      <c r="O41" s="5">
+        <v>2.4694577912838599E-2</v>
+      </c>
+      <c r="P41" s="5">
+        <v>2.48559342758627E-2</v>
+      </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -17571,7 +19156,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -17600,7 +19185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V436"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -17612,49 +19197,49 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>31</v>
       </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
       <c r="U1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V1">
         <f>AVERAGE(K:K)</f>
@@ -17663,7 +19248,7 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5">
         <v>0.99644676813178201</v>
@@ -17706,7 +19291,7 @@
         <v>0.49320000000000003</v>
       </c>
       <c r="U2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V2">
         <f>AVERAGE(L:L)</f>
@@ -17715,7 +19300,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5">
         <v>0.99959621907645901</v>
@@ -17758,7 +19343,7 @@
         <v>0.51629999999999998</v>
       </c>
       <c r="U3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V3">
         <f>AVERAGE(M:M)</f>
@@ -17767,7 +19352,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5">
         <v>0.99980094939376396</v>
@@ -17810,7 +19395,7 @@
         <v>0.98899999999999999</v>
       </c>
       <c r="U4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V4">
         <f>AVERAGE(N:N)</f>
@@ -17819,7 +19404,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5">
         <v>0.99776364471115497</v>
@@ -17862,7 +19447,7 @@
         <v>0.46729999999999999</v>
       </c>
       <c r="U5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V5">
         <f>AVERAGE(O:O)</f>
@@ -17871,7 +19456,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5">
         <v>0.98631225686810897</v>
@@ -17914,7 +19499,7 @@
         <v>0.43759999999999999</v>
       </c>
       <c r="U6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V6">
         <f>AVERAGE(P:P)</f>
@@ -17923,7 +19508,7 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5">
         <v>0.99942239711541803</v>
@@ -17966,7 +19551,7 @@
         <v>0.47449999999999998</v>
       </c>
       <c r="U7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V7">
         <f>AVERAGE(Q:Q)</f>
@@ -17975,7 +19560,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5">
         <v>0.98483444286444999</v>
@@ -18018,7 +19603,7 @@
         <v>0.44469999999999998</v>
       </c>
       <c r="U8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V8">
         <f>AVERAGE(R:R)</f>
@@ -18027,7 +19612,7 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5">
         <v>0.99254602929234803</v>
@@ -18070,7 +19655,7 @@
         <v>0.35360000000000003</v>
       </c>
       <c r="U9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V9">
         <f>AVERAGE(S:S)</f>
@@ -18079,7 +19664,7 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5">
         <v>0.99907223486808305</v>
@@ -30491,7 +32076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q2188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -30502,34 +32087,34 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q1">
         <f>AVERAGE(K:K)</f>
@@ -30538,7 +32123,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5">
         <v>0.99207141080852101</v>
@@ -30566,7 +32151,7 @@
         <v>0.6956</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2">
         <f>AVERAGE(L:L)</f>
@@ -30575,7 +32160,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5">
         <v>0.99473251008163299</v>
@@ -30603,7 +32188,7 @@
         <v>0.28749999999999998</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q3">
         <f>AVERAGE(M:M)</f>
@@ -30612,7 +32197,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5">
         <v>0.99624330283762597</v>
@@ -30640,7 +32225,7 @@
         <v>0.4017</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4">
         <f>AVERAGE(N:N)</f>
@@ -30649,7 +32234,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5">
         <v>0.999967936595893</v>
@@ -35642,17 +37227,17 @@
     </row>
     <row r="437" spans="12:14">
       <c r="M437" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="438" spans="12:14">
       <c r="M438" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="439" spans="12:14">
       <c r="M439" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="440" spans="12:14">
@@ -37832,17 +39417,17 @@
     </row>
     <row r="875" spans="13:13">
       <c r="M875" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="876" spans="13:13">
       <c r="M876" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="877" spans="13:13">
       <c r="M877" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="878" spans="13:13">
@@ -40022,17 +41607,17 @@
     </row>
     <row r="1313" spans="13:13">
       <c r="M1313" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1314" spans="13:13">
       <c r="M1314" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="1315" spans="13:13">
       <c r="M1315" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="1316" spans="13:13">
@@ -42212,17 +43797,17 @@
     </row>
     <row r="1751" spans="13:13">
       <c r="M1751" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1752" spans="13:13">
       <c r="M1752" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="1753" spans="13:13">
       <c r="M1753" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="1754" spans="13:13">
@@ -44419,31 +46004,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
@@ -45133,31 +46718,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">

</xml_diff>

<commit_message>
chr 8,7,11 for 500kb resolution
</commit_message>
<xml_diff>
--- a/Results/ResultsTest1.xlsx
+++ b/Results/ResultsTest1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ParticleChromo3D\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F93DC-A968-4A9C-B645-29BD4F250E22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18504A8A-1BEE-4B2B-95DD-73CB049654F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6345" yWindow="3345" windowWidth="25215" windowHeight="15435" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="49">
   <si>
     <t>alpha</t>
   </si>
@@ -221,6 +221,18 @@
   <si>
     <t xml:space="preserve">ParticleChromo3D </t>
   </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Spearman</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
 </sst>
 </file>
 
@@ -335,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -380,6 +392,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -395,7 +418,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -441,6 +464,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4344,6 +4371,20 @@
         <c:showVertBorder val="1"/>
         <c:showOutline val="1"/>
         <c:showKeys val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
       </c:dTable>
       <c:spPr>
         <a:noFill/>
@@ -4435,13 +4476,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>SCC at Different Local</a:t>
+              <a:t>SCC at Different Local Confidences</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Confidences vs Global Confidence</a:t>
+              <a:t> vs Global Confidence</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4490,7 +4534,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4507,17 +4551,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Coeffecient_test!$T$1:$V$1</c:f>
+              <c:f>Coeffecient_test!$T$1:$AC$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -4525,25 +4590,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Coeffecient_test!$T$2:$V$2</c:f>
+              <c:f>Coeffecient_test!$T$2:$AC$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>6.6322647822716504E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7.5435310430800803E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.101530293795098</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.105514742244953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1732378554561405E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.128296807618589</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37213812496097398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99377130598532104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99814338881887299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99216247324951001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3353-433E-92B9-8B98FE1A49EE}"/>
+              <c16:uniqueId val="{00000000-0CF4-4932-9CF9-F8BA9D6A8ED7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4556,7 +4642,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4573,17 +4659,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Coeffecient_test!$T$1:$V$1</c:f>
+              <c:f>Coeffecient_test!$T$1:$AC$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -4591,25 +4698,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Coeffecient_test!$T$3:$V$3</c:f>
+              <c:f>Coeffecient_test!$T$3:$AC$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>8.1732378554561405E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.128296807618589</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.37213812496097398</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>7.5435310430800803E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.101530293795098</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.105514742244953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3353-433E-92B9-8B98FE1A49EE}"/>
+              <c16:uniqueId val="{00000001-0CF4-4932-9CF9-F8BA9D6A8ED7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4622,7 +4729,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4639,17 +4746,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Coeffecient_test!$T$1:$V$1</c:f>
+              <c:f>Coeffecient_test!$T$1:$AC$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -4657,30 +4785,116 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Coeffecient_test!$T$4:$V$4</c:f>
+              <c:f>Coeffecient_test!$T$4:$AC$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.99377130598532104</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99672801553520796</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99620063830389705</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>8.1732378554561405E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.128296807618589</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.37213812496097398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3353-433E-92B9-8B98FE1A49EE}"/>
+              <c16:uniqueId val="{00000002-0CF4-4932-9CF9-F8BA9D6A8ED7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coeffecient_test!$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$1:$AC$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Coeffecient_test!$T$5:$AC$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>0.99377130598532104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99672801553520796</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99620063830389705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0CF4-4932-9CF9-F8BA9D6A8ED7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4690,11 +4904,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1143806703"/>
-        <c:axId val="1143802543"/>
+        <c:axId val="1202630415"/>
+        <c:axId val="1202637903"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1143806703"/>
+        <c:axId val="1202630415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4721,8 +4935,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Global Confidence</a:t>
+                  <a:t>Global</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Confidence</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4792,7 +5011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1143802543"/>
+        <c:crossAx val="1202637903"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4800,7 +5019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1143802543"/>
+        <c:axId val="1202637903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4876,7 +5095,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4907,7 +5126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1143806703"/>
+        <c:crossAx val="1202630415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5038,42 +5257,52 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
+            <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>SCC Average Between 30 Structures per Chromosome </a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>SCC</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> by Global Confidence</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>at Local Confidence 0.3</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5083,7 +5312,28 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -5095,93 +5345,123 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coeffecient_test!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Spearman</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="4472C4"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'consistency-1MB'!$A$2:$A$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Coeffecient_test!$N$1:$N$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Coeffecient_test!$N$2:$N$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>chr1</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>chr2</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>chr5</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>chr10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>chr15</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>chr19</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>chr20</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>chr21</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>chr22</c:v>
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'consistency-1MB'!$B$2:$B$10</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Coeffecient_test!$P$2:$P$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Coeffecient_test!$P$3:$P$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.99644676813178201</c:v>
+                  <c:v>7.5435310430800803E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99959621907645901</c:v>
+                  <c:v>0.101530293795098</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99980094939376396</c:v>
+                  <c:v>0.105514742244953</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99776364471115497</c:v>
+                  <c:v>8.1732378554561405E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98631225686810897</c:v>
+                  <c:v>0.128296807618589</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99942239711541803</c:v>
+                  <c:v>0.37213812496097398</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98483444286444999</c:v>
+                  <c:v>0.99377130598532104</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99254602929234803</c:v>
+                  <c:v>0.99814338881887299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99907223486808305</c:v>
+                  <c:v>0.99216247324951001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-146B-4153-9D9D-4FB80D337464}"/>
+              <c16:uniqueId val="{00000000-460D-42C7-A7C1-3657A37482EB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -5191,11 +5471,117 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="514553200"/>
-        <c:axId val="514562352"/>
+        <c:axId val="1161682559"/>
+        <c:axId val="1161687551"/>
       </c:barChart>
+      <c:catAx>
+        <c:axId val="1161682559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Global Confidence</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1161687551"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="514562352"/>
+        <c:axId val="1161687551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5204,47 +5590,39 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9528" cap="flat">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
+                <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>SCC</a:t>
                 </a:r>
               </a:p>
@@ -5256,9 +5634,30 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5267,184 +5666,111 @@
           <a:ln>
             <a:noFill/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
+            <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="514553200"/>
+        <c:crossAx val="1161682559"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:catAx>
-        <c:axId val="514553200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Chromosome</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="0"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9528" cap="flat">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
+            <a:pPr rtl="0">
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Calibri"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="514562352"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
       </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9528" cap="flat">
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
   <c:txPr>
-    <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+    <a:bodyPr/>
     <a:lstStyle/>
     <a:p>
-      <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-        <a:lnSpc>
-          <a:spcPct val="100000"/>
-        </a:lnSpc>
-        <a:spcBef>
-          <a:spcPts val="0"/>
-        </a:spcBef>
-        <a:spcAft>
-          <a:spcPts val="0"/>
-        </a:spcAft>
-        <a:tabLst/>
-        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Calibri"/>
-        </a:defRPr>
+      <a:pPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -5956,6 +6282,960 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PCC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> by Global Confidence</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>at Local Confidence 0.3</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coeffecient_test!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pearson</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Coeffecient_test!$N$1:$N$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Coeffecient_test!$N$2:$N$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Coeffecient_test!$O$2:$O$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Coeffecient_test!$O$3:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.5653206420151904E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.124147814037815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12666432036703101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10290602252389799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17208333762880801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45620814069263199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99429792923667704</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99820301162700098</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99298009111866203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB79-4376-B0A2-2489FCBDF3C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1161682559"/>
+        <c:axId val="1161687551"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1161682559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Global Confidence</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1161687551"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1161687551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PCC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1161682559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="0"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>SCC Average Between 30 Structures per Chromosome </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'consistency-1MB'!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>chr1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>chr2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chr5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>chr10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>chr15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>chr19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>chr20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>chr21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>chr22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'consistency-1MB'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.99644676813178201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99959621907645901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99980094939376396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99776364471115497</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98631225686810897</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99942239711541803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98483444286444999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99254602929234803</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99907223486808305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-146B-4153-9D9D-4FB80D337464}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="514553200"/>
+        <c:axId val="514562352"/>
+      </c:barChart>
+      <c:valAx>
+        <c:axId val="514562352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9528" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>SCC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514553200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="514553200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Chromosome</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9528" cap="flat">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514562352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9528" cap="flat">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+        <a:lnSpc>
+          <a:spcPct val="100000"/>
+        </a:lnSpc>
+        <a:spcBef>
+          <a:spcPts val="0"/>
+        </a:spcBef>
+        <a:spcAft>
+          <a:spcPts val="0"/>
+        </a:spcAft>
+        <a:tabLst/>
+        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Calibri"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
     <c:title>
@@ -6374,7 +7654,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6797,7 +8077,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7191,7 +8471,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7584,7 +8864,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7977,7 +9257,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9227,7 +10507,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -14513,6 +15793,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -15017,6 +16377,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15531,7 +17897,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16566,10 +18932,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>133346</xdr:rowOff>
+      <xdr:rowOff>76196</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6121816" cy="3443081"/>
     <xdr:graphicFrame macro="">
@@ -16597,23 +18963,23 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>633411</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2260126E-C95B-43B3-A23D-AFF637E86EE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E723C4D-CE99-453D-96EC-5D206DAA2891}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16626,6 +18992,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7DD4FFE-8548-4B6E-B07D-5B078056C58B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FCF2759-42D4-49CC-B3A6-55AF908CC5A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -18175,10 +20615,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:V83"/>
+  <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18187,7 +20627,7 @@
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -18216,28 +20656,49 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
+        <v>45</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="T1">
+        <v>0.1</v>
+      </c>
+      <c r="U1">
+        <v>0.4</v>
+      </c>
+      <c r="V1">
+        <v>0.7</v>
+      </c>
+      <c r="W1">
+        <v>1</v>
+      </c>
+      <c r="X1">
+        <v>1.3</v>
+      </c>
+      <c r="Y1">
+        <v>1.6</v>
+      </c>
+      <c r="Z1">
+        <v>1.9</v>
+      </c>
+      <c r="AA1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="U1">
+      <c r="AB1">
         <v>2.5</v>
       </c>
-      <c r="V1">
+      <c r="AC1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -18266,35 +20727,63 @@
         <v>0.99837607469027201</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="M2">
+      <c r="M2" s="23">
         <v>0.3</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="23">
         <v>0.1</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="26">
         <v>8.3145397809773702E-2</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="26">
         <v>6.6322647822716504E-2</v>
       </c>
-      <c r="S2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="T2" s="5">
+      <c r="S2">
+        <v>0.3</v>
+      </c>
+      <c r="T2" s="6">
+        <f>P2</f>
+        <v>6.6322647822716504E-2</v>
+      </c>
+      <c r="U2" s="6">
         <f>P3</f>
         <v>7.5435310430800803E-2</v>
       </c>
-      <c r="U2" s="5">
+      <c r="V2" s="6">
         <f>P4</f>
         <v>0.101530293795098</v>
       </c>
-      <c r="V2" s="5">
+      <c r="W2" s="6">
         <f>P5</f>
         <v>0.105514742244953</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="X2" s="6">
+        <f>P6</f>
+        <v>8.1732378554561405E-2</v>
+      </c>
+      <c r="Y2" s="6">
+        <f>P7</f>
+        <v>0.128296807618589</v>
+      </c>
+      <c r="Z2" s="6">
+        <f>P8</f>
+        <v>0.37213812496097398</v>
+      </c>
+      <c r="AA2" s="6">
+        <f>P9</f>
+        <v>0.99377130598532104</v>
+      </c>
+      <c r="AB2" s="6">
+        <f>P10</f>
+        <v>0.99814338881887299</v>
+      </c>
+      <c r="AC2" s="6">
+        <f>P11</f>
+        <v>0.99216247324951001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="7">
         <v>0.3</v>
       </c>
@@ -18337,114 +20826,129 @@
       <c r="P3" s="1">
         <v>7.5435310430800803E-2</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AA3" s="5">
+        <f>P3</f>
+        <v>7.5435310430800803E-2</v>
+      </c>
+      <c r="AB3" s="5">
+        <f>P4</f>
+        <v>0.101530293795098</v>
+      </c>
+      <c r="AC3" s="5">
+        <f>P5</f>
+        <v>0.105514742244953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4">
+        <v>0.6</v>
+      </c>
+      <c r="B4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.99700142156094396</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.99682016310779797</v>
+      </c>
+      <c r="E4" s="1">
+        <v>25.909417066332399</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.99845046503135004</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.99837607469027201</v>
+      </c>
+      <c r="M4">
+        <v>0.3</v>
+      </c>
+      <c r="N4">
         <v>0.7</v>
       </c>
-      <c r="T3" s="5">
+      <c r="O4" s="1">
+        <v>0.124147814037815</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.101530293795098</v>
+      </c>
+      <c r="S4">
+        <v>0.7</v>
+      </c>
+      <c r="AA4" s="5">
         <f>P6</f>
         <v>8.1732378554561405E-2</v>
       </c>
-      <c r="U3" s="5">
+      <c r="AB4" s="5">
         <f>P7</f>
         <v>0.128296807618589</v>
       </c>
-      <c r="V3" s="5">
+      <c r="AC4" s="5">
         <f>P8</f>
         <v>0.37213812496097398</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
-      <c r="A4">
-        <v>0.6</v>
-      </c>
-      <c r="B4">
+    <row r="5" spans="1:29">
+      <c r="A5">
+        <v>0.9</v>
+      </c>
+      <c r="B5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C4" s="9">
-        <v>0.99700142156094396</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.99682016310779797</v>
-      </c>
-      <c r="E4" s="1">
-        <v>25.909417066332399</v>
-      </c>
-      <c r="G4">
-        <v>0.6</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="C5" s="1">
+        <v>0.99649379196631505</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.99621976052930705</v>
+      </c>
+      <c r="E5" s="1">
+        <v>26.7675591382114</v>
+      </c>
+      <c r="G5">
+        <v>0.9</v>
+      </c>
+      <c r="H5" s="1">
         <v>2.5</v>
       </c>
-      <c r="I4" s="5">
-        <v>0.99845046503135004</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.99837607469027201</v>
-      </c>
-      <c r="M4">
+      <c r="M5">
         <v>0.3</v>
       </c>
-      <c r="N4">
-        <v>0.7</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0.124147814037815</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.101530293795098</v>
-      </c>
-      <c r="S4">
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.12666432036703101</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.105514742244953</v>
+      </c>
+      <c r="S5">
         <v>0.9</v>
       </c>
-      <c r="T4" s="5">
+      <c r="AA5" s="5">
         <f>P9</f>
         <v>0.99377130598532104</v>
       </c>
-      <c r="U4" s="5">
-        <f>P19</f>
+      <c r="AB5" s="5">
+        <f>P20</f>
         <v>0.99672801553520796</v>
       </c>
-      <c r="V4" s="5">
-        <f>P20</f>
+      <c r="AC5" s="5">
+        <f>P21</f>
         <v>0.99620063830389705</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
-      <c r="A5">
-        <v>0.9</v>
-      </c>
-      <c r="B5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.99649379196631505</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.99621976052930705</v>
-      </c>
-      <c r="E5" s="1">
-        <v>26.7675591382114</v>
-      </c>
-      <c r="G5">
-        <v>0.9</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="M5">
-        <v>0.3</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0.12666432036703101</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0.105514742244953</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>1.2</v>
       </c>
@@ -18479,7 +20983,7 @@
         <v>8.1732378554561405E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -18514,7 +21018,7 @@
         <v>0.128296807618589</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>1.9</v>
       </c>
@@ -18549,7 +21053,7 @@
         <v>0.37213812496097398</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>0.3</v>
       </c>
@@ -18584,7 +21088,7 @@
         <v>0.99377130598532104</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>0.3</v>
       </c>
@@ -18621,14 +21125,14 @@
       <c r="N10">
         <v>2.5</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="11">
         <v>0.99820301162700098</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="11">
         <v>0.99814338881887299</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>0.3</v>
       </c>
@@ -18664,7 +21168,7 @@
         <v>0.99216247324951001</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>0.3</v>
       </c>
@@ -18686,16 +21190,20 @@
       <c r="H12" s="1">
         <v>2.8</v>
       </c>
-      <c r="M12" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="N12" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="M12" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>0.3</v>
       </c>
@@ -18717,14 +21225,16 @@
       <c r="H13" s="1">
         <v>2.8</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="21">
         <v>0.5</v>
       </c>
-      <c r="N13">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="N13" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>0.3</v>
       </c>
@@ -18750,10 +21260,10 @@
         <v>0.5</v>
       </c>
       <c r="N14">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>0.3</v>
       </c>
@@ -18779,10 +21289,10 @@
         <v>0.5</v>
       </c>
       <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>0.3</v>
       </c>
@@ -18802,7 +21312,7 @@
         <v>0.5</v>
       </c>
       <c r="N16">
-        <v>1.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -18825,7 +21335,7 @@
         <v>0.5</v>
       </c>
       <c r="N17">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -18848,83 +21358,89 @@
         <v>0.5</v>
       </c>
       <c r="N18">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="M19" s="22">
         <v>0.5</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="M20" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N20" s="22">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O20" s="22">
         <v>0.99689891449684798</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P20" s="22">
         <v>0.99672801553520796</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="M20">
+    <row r="21" spans="1:16">
+      <c r="M21">
         <v>0.5</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>2.5</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O21" s="5">
         <v>0.99659953493572395</v>
       </c>
-      <c r="P20" s="5">
+      <c r="P21" s="5">
         <v>0.99620063830389705</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="M21" s="5">
+    <row r="22" spans="1:16">
+      <c r="M22" s="5">
         <v>0.5</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>2.8</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O22" s="5">
         <v>2.5800494948756799E-2</v>
       </c>
-      <c r="P21" s="5">
+      <c r="P22" s="5">
         <v>1.7421163822083498E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="M22" s="23">
+    <row r="23" spans="1:16">
+      <c r="M23" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="O23" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="P23" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="M24" s="23">
         <v>0.7</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N24" s="23">
         <v>0.1</v>
       </c>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="M23">
-        <v>0.7</v>
-      </c>
-      <c r="N23">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="M24">
-        <v>0.7</v>
-      </c>
-      <c r="N24">
-        <v>0.7</v>
-      </c>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
     </row>
     <row r="25" spans="1:16">
       <c r="M25">
         <v>0.7</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -18932,7 +21448,7 @@
         <v>0.7</v>
       </c>
       <c r="N26">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -18940,7 +21456,7 @@
         <v>0.7</v>
       </c>
       <c r="N27">
-        <v>1.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -18948,21 +21464,15 @@
         <v>0.7</v>
       </c>
       <c r="N28">
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="M29">
         <v>0.7</v>
       </c>
-      <c r="N29" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O29" s="5">
-        <v>0.99844535101737397</v>
-      </c>
-      <c r="P29" s="5">
-        <v>0.99846462103771205</v>
+      <c r="N29">
+        <v>1.6</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -18970,62 +21480,74 @@
         <v>0.7</v>
       </c>
       <c r="N30">
-        <v>2.5</v>
-      </c>
-      <c r="O30" s="5">
-        <v>1.6894316798075602E-2</v>
-      </c>
-      <c r="P30" s="5">
-        <v>1.26692786830521E-2</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="M31">
         <v>0.7</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O31" s="5">
+        <v>0.99844535101737397</v>
+      </c>
+      <c r="P31" s="5">
+        <v>0.99846462103771205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="M32">
+        <v>0.7</v>
+      </c>
+      <c r="N32">
+        <v>2.5</v>
+      </c>
+      <c r="O32" s="5">
+        <v>1.6894316798075602E-2</v>
+      </c>
+      <c r="P32" s="5">
+        <v>1.26692786830521E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="13:22">
+      <c r="M33">
+        <v>0.7</v>
+      </c>
+      <c r="N33">
         <v>2.8</v>
       </c>
-      <c r="O31" s="5">
+      <c r="O33" s="5">
         <v>4.8827333114792197E-2</v>
       </c>
-      <c r="P31" s="5">
+      <c r="P33" s="5">
         <v>3.7434444673984997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="M32" s="23">
+    <row r="34" spans="13:22">
+      <c r="M34" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="O34" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="P34" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="13:22">
+      <c r="M35" s="23">
         <v>0.9</v>
       </c>
-      <c r="N32" s="23">
+      <c r="N35" s="23">
         <v>0.1</v>
       </c>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="13:22">
-      <c r="M33" s="24">
-        <v>0.9</v>
-      </c>
-      <c r="N33">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="34" spans="13:22">
-      <c r="M34" s="24">
-        <v>0.9</v>
-      </c>
-      <c r="N34">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="35" spans="13:22">
-      <c r="M35" s="24">
-        <v>0.9</v>
-      </c>
-      <c r="N35">
-        <v>1</v>
-      </c>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
@@ -19035,7 +21557,7 @@
         <v>0.9</v>
       </c>
       <c r="N36">
-        <v>1.3</v>
+        <v>0.4</v>
       </c>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
@@ -19045,7 +21567,7 @@
         <v>0.9</v>
       </c>
       <c r="N37">
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
@@ -19055,48 +21577,72 @@
         <v>0.9</v>
       </c>
       <c r="N38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="13:22">
+      <c r="M39" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N39">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="40" spans="13:22">
+      <c r="M40" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N40">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="41" spans="13:22">
+      <c r="M41" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="N41">
         <v>1.9</v>
       </c>
     </row>
-    <row r="39" spans="13:22">
-      <c r="M39">
+    <row r="42" spans="13:22">
+      <c r="M42">
         <v>0.9</v>
       </c>
-      <c r="N39" s="5">
+      <c r="N42" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O39" s="5">
+      <c r="O42" s="5">
         <v>0.99879633533495804</v>
       </c>
-      <c r="P39" s="5">
+      <c r="P42" s="5">
         <v>0.99868591146533103</v>
       </c>
     </row>
-    <row r="40" spans="13:22">
-      <c r="M40">
+    <row r="43" spans="13:22">
+      <c r="M43">
         <v>0.9</v>
       </c>
-      <c r="N40">
+      <c r="N43">
         <v>2.5</v>
       </c>
-      <c r="O40" s="5">
+      <c r="O43" s="5">
         <v>2.2597942669239202E-2</v>
       </c>
-      <c r="P40" s="5">
+      <c r="P43" s="5">
         <v>2.0561717472259499E-2</v>
       </c>
     </row>
-    <row r="41" spans="13:22">
-      <c r="M41">
+    <row r="44" spans="13:22">
+      <c r="M44">
         <v>0.9</v>
       </c>
-      <c r="N41">
+      <c r="N44">
         <v>2.8</v>
       </c>
-      <c r="O41" s="5">
+      <c r="O44" s="5">
         <v>2.4694577912838599E-2</v>
       </c>
-      <c r="P41" s="5">
+      <c r="P44" s="5">
         <v>2.48559342758627E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
results hsa and fin pin .5 local
</commit_message>
<xml_diff>
--- a/Results/ResultsTest1.xlsx
+++ b/Results/ResultsTest1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ParticleChromo3D\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85E0145-3EDD-4D0A-BB8D-D6BCFF325336}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C286121-77AC-4AD3-B0D6-9C25D3AD5F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="3345" windowWidth="25215" windowHeight="15435" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="3345" windowWidth="25215" windowHeight="15435" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameterChoiceForBestAlpha" sheetId="1" r:id="rId1"/>
@@ -5601,6 +5601,9 @@
                 <c:pt idx="5">
                   <c:v>0.183544275958646</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99033647609276299</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>0.99672801553520796</c:v>
                 </c:pt>
@@ -6611,6 +6614,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.26040022941611102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99128783527737097</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.99689891449684798</c:v>
@@ -26180,7 +26186,7 @@
   <dimension ref="A1:AC83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N10" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -26963,6 +26969,12 @@
       </c>
       <c r="N19">
         <v>1.9</v>
+      </c>
+      <c r="O19">
+        <v>0.99128783527737097</v>
+      </c>
+      <c r="P19">
+        <v>0.99033647609276299</v>
       </c>
     </row>
     <row r="20" spans="1:16">

</xml_diff>

<commit_message>
remove hsa update swarmsize
</commit_message>
<xml_diff>
--- a/Results/ResultsTest1.xlsx
+++ b/Results/ResultsTest1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ParticleChromo3D\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F98EF55-AD49-41B4-8DF9-9D8628DD4CAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EF011E-4BDC-48A0-A3F8-F2E3B7BF9D63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="3345" windowWidth="25215" windowHeight="15435" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12615" yWindow="2175" windowWidth="25215" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameterChoiceForBestAlpha" sheetId="1" r:id="rId1"/>
@@ -34,35 +34,17 @@
     <definedName name="_xlchart.v1.15" hidden="1">'consistency-1MB'!$R$2:$R$436</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">'consistency-1MB'!$S$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">'consistency-1MB'!$S$2:$S$436</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'consistency-1MB'!$K$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'consistency-1MB'!$K$2:$K$436</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'consistency-500kb'!$K$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'consistency-500kb'!$K$2:$K$2188</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'consistency-1MB'!$L$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'consistency-1MB'!$L$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'consistency-1MB'!$L$2:$L$436</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'consistency-1MB'!$M$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'consistency-1MB'!$M$2:$M$436</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'consistency-1MB'!$N$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'consistency-1MB'!$N$2:$N$436</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'consistency-1MB'!$O$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'consistency-1MB'!$O$2:$O$436</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'consistency-1MB'!$P$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'consistency-1MB'!$P$2:$P$436</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'consistency-500kb'!$L$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'consistency-500kb'!$L$2:$L$2188</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'consistency-500kb'!$M$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'consistency-500kb'!$M$2:$M$2188</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'consistency-500kb'!$N$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'consistency-500kb'!$N$2:$N$2188</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'consistency-1MB'!$L$2:$L$436</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'consistency-1MB'!$Q$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'consistency-1MB'!$Q$2:$Q$436</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'consistency-1MB'!$R$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'consistency-1MB'!$R$2:$R$436</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'consistency-1MB'!$S$1</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'consistency-1MB'!$S$2:$S$436</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'consistency-500kb'!$K$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'consistency-500kb'!$K$2:$K$2188</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'consistency-500kb'!$L$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'consistency-500kb'!$L$2:$L$2188</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'consistency-1MB'!$M$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'consistency-500kb'!$M$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'consistency-500kb'!$M$2:$M$2188</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'consistency-500kb'!$N$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'consistency-500kb'!$N$2:$N$2188</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'consistency-1MB'!$M$2:$M$436</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'consistency-1MB'!$N$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'consistency-1MB'!$N$2:$N$436</definedName>
@@ -4646,7 +4628,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -15218,10 +15199,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>swarmSizeTest!$A$2:$A$4</c:f>
+              <c:f>swarmSizeTest!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -15229,6 +15210,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -15236,18 +15220,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>swarmSizeTest!$B$2:$B$4</c:f>
+              <c:f>swarmSizeTest!$B$2:$B$5</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>25.329329113090999</c:v>
+                  <c:v>381.89804409596297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.597125906735901</c:v>
+                  <c:v>92.419394459013404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.0155616133415</c:v>
+                  <c:v>166.26041119392599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.283251665744199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15334,7 +15321,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15475,6 +15462,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -15616,10 +15609,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>swarmSizeTest!$A$2:$A$4</c:f>
+              <c:f>swarmSizeTest!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -15627,6 +15620,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -15634,18 +15630,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>swarmSizeTest!$C$2:$C$4</c:f>
+              <c:f>swarmSizeTest!$C$2:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0000000</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.99632680940065599</c:v>
+                  <c:v>0.99690667592065496</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99982768835176195</c:v>
+                  <c:v>0.99919536245080898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99998240332545996</c:v>
+                  <c:v>0.99895894342573399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99984288605976002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15732,7 +15731,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0000000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15873,6 +15872,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -16014,10 +16019,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>swarmSizeTest!$A$2:$A$4</c:f>
+              <c:f>swarmSizeTest!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -16025,6 +16030,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -16032,18 +16040,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>swarmSizeTest!$D$2:$D$4</c:f>
+              <c:f>swarmSizeTest!$D$2:$D$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0000000</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.99575660753782902</c:v>
+                  <c:v>0.996975446948688</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99980107722594902</c:v>
+                  <c:v>0.99920804353688097</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99997923148544599</c:v>
+                  <c:v>0.99894782884359501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99982462728822397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16130,7 +16141,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0000000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -16271,6 +16282,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -16412,10 +16429,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>swarmSizeTest!$A$2:$A$4</c:f>
+              <c:f>swarmSizeTest!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -16423,6 +16440,9 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -16430,18 +16450,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>swarmSizeTest!$E$2:$E$4</c:f>
+              <c:f>swarmSizeTest!$E$2:$E$5</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.0000">
                   <c:v>170.06859517097499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>415.267109394074</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>660.24529170990002</c:v>
+                  <c:v>519.625492811203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>758.22447657585099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1021.04460740089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16669,6 +16692,12 @@
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln w="9528">
@@ -17561,47 +17590,47 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.29</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.31</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.33</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.35</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -17639,7 +17668,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E74A45CE-B0CE-4284-AD37-4930D0C01BCC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>chr1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17652,7 +17681,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4609CE68-5C56-4848-9F7F-D5A847B5B531}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>chr2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17665,7 +17694,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B572AA01-5165-4463-9556-6071969C41E6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>chr5</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17678,7 +17707,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{0C22D4F5-4BCE-466F-A466-25E8A48B3543}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.24</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>chr10</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17691,7 +17720,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8CB4A5A0-6872-4707-A7D7-7DC65CC83719}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.26</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>chr15</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17704,7 +17733,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B7B94A64-8346-49DD-9086-43559FCFD78D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>chr19</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17717,7 +17746,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D3994CC7-33C9-4B5A-B63C-1071FA6518E9}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.30</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>chr20</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17730,7 +17759,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{BBDBC415-1A60-4213-BA90-2D8510942363}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.32</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>chr21</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17743,7 +17772,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{380E1564-8E15-44AC-BDEF-5F3A534B83E8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.34</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>chr22</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17822,22 +17851,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.39</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -17875,7 +17904,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FC0FDC28-34D3-4A75-A532-D3429BECE732}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.36</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>chr1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17888,7 +17917,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FDF954FF-C90D-448A-BAC7-9EB7101C5083}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.38</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>chr10</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17901,7 +17930,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{37A695BD-6086-4712-9A72-01FE7C456FFF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>chr19</cx:v>
             </cx:txData>
           </cx:tx>
@@ -17914,7 +17943,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{588D971C-E56B-4A45-8E9E-CFAF2A37CD1E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.42</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>chr22</cx:v>
             </cx:txData>
           </cx:tx>
@@ -25818,7 +25847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -25847,14 +25878,14 @@
       <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>25.329329113090999</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.99632680940065599</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.99575660753782902</v>
+      <c r="B2" s="5">
+        <v>381.89804409596297</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.99690667592065496</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.996975446948688</v>
       </c>
       <c r="E2" s="3">
         <v>170.06859517097499</v>
@@ -25864,41 +25895,53 @@
       <c r="A3">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
-        <v>24.597125906735901</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.99982768835176195</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.99980107722594902</v>
-      </c>
-      <c r="E3" s="3">
-        <v>415.267109394074</v>
+      <c r="B3" s="5">
+        <v>92.419394459013404</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.99919536245080898</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.99920804353688097</v>
+      </c>
+      <c r="E3" s="5">
+        <v>519.625492811203</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5">
+        <v>166.26041119392599</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.99895894342573399</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.99894782884359501</v>
+      </c>
+      <c r="E4" s="5">
+        <v>758.22447657585099</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
         <v>20</v>
       </c>
-      <c r="B4" s="1">
-        <v>26.0155616133415</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.99998240332545996</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.99997923148544599</v>
-      </c>
-      <c r="E4" s="4">
-        <v>660.24529170990002</v>
-      </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="5">
+        <v>20.283251665744199</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.99984288605976002</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.99982462728822397</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1021.04460740089</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="B6" s="1"/>
@@ -25977,12 +26020,12 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -26336,7 +26379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P25" workbookViewId="0">
+    <sheetView topLeftCell="P25" workbookViewId="0">
       <selection activeCell="AD65" sqref="AD65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
begin add 15sc to gm analysis
</commit_message>
<xml_diff>
--- a/Results/ResultsTest1.xlsx
+++ b/Results/ResultsTest1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ParticleChromo3D\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C778DAC8-B62F-4224-9C1B-4E14819B62A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E93F60-98DB-4E12-A5A9-429EAE9413E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12615" yWindow="2175" windowWidth="25215" windowHeight="15435" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12615" yWindow="2175" windowWidth="25215" windowHeight="15435" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameterChoiceForBestAlpha" sheetId="1" r:id="rId1"/>

</xml_diff>